<commit_message>
aregle presupuesto de casa de fin de semana y visualizacion de reservas para esta propuedad
</commit_message>
<xml_diff>
--- a/CasosDeUso/CasosDeUso.xlsx
+++ b/CasosDeUso/CasosDeUso.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOCUMENTOS\TECNICATURA\Laboratorio ll\TP2\Booking\Casos de uso\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOCUMENTOS\TECNICATURA\Laboratorio ll\TP2\Booking\CasosDeUso\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -143,6 +143,52 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>Curso Alternativo 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: El usuario cancela el proceso en cualquier momento</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Curso Alternativo 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: 4- No existen propiedades que se adecuen al filtro de busqueda</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Excepciones</t>
     </r>
     <r>
@@ -156,56 +202,10 @@
       <t xml:space="preserve">: 
 7- No se puede seleccionar esta fecha
 9- Debe indicar un nombre
-10- Debe indicar un DNI
-11- Debe indicar un telefono
-12- Debe indicar la direccion
+9- Debe indicar un DNI
+9- Debe indicar un telefono
+9- Debe indicar la direccion
 </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Curso Alternativo 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: El usuario cancela el proceso en cualquier momento</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Curso Alternativo 2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: 4- No existen propiedades que se adecuen al filtro de busqueda</t>
     </r>
   </si>
 </sst>
@@ -297,11 +297,24 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -309,19 +322,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -604,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,115 +614,115 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="7"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="6"/>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="6"/>
     </row>
     <row r="5" spans="2:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="8"/>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="9"/>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="2"/>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="6"/>
-      <c r="C9" s="6" t="s">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="6"/>
+      <c r="C10" s="2"/>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="6"/>
-      <c r="C11" s="6" t="s">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="6"/>
+      <c r="C12" s="2"/>
     </row>
     <row r="13" spans="2:3" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B13" s="6"/>
-      <c r="C13" s="6" t="s">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="6"/>
+      <c r="C14" s="2"/>
     </row>
     <row r="15" spans="2:3" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B15" s="6"/>
-      <c r="C15" s="6" t="s">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="2:3" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="6"/>
+      <c r="C16" s="2"/>
     </row>
     <row r="17" spans="2:14" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="N17" s="3"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="N17" s="9"/>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="2"/>
+      <c r="C19" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>